<commit_message>
Se consideraron casos rezagados y volvimos a ejecutar
</commit_message>
<xml_diff>
--- a/VRAI2026/cursos2026/formulario_single_1.xlsx
+++ b/VRAI2026/cursos2026/formulario_single_1.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X7"/>
+  <dimension ref="A1:X8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -547,7 +547,7 @@
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t>Convenio Específico</t>
+          <t>Convenio específico</t>
         </is>
       </c>
       <c r="X1" s="1" t="inlineStr">
@@ -564,57 +564,57 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Ane Garmendia Errasti</t>
+          <t>Cécile Juvé</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://www.dropbox.com/scl/fi/bgf9c6gpcjzwu2cf79p0o/Expediente-academico.pdf?rlkey=zshjetl3jxmbpyf7hev609cry&amp;st=5kqylkk5&amp;dl=0</t>
+          <t>https://www.dropbox.com/scl/fi/2ps9xq5w068xrjdpppv3b/certificados_notas_universidad_origen_JUVE_Cecile.pdf?rlkey=k6tdbssxu60ujapldrt2b6g6d&amp;st=qktkmrtu&amp;dl=0</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1185535</t>
+          <t>1185373</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>anegarmendiaerrasti@gmail.com</t>
+          <t>cecile.juve@sorbonne-nouvelle.fr</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>anegarmendiaerrasti@gmail.com</t>
+          <t>cecile.juve@sorbonne-nouvelle.fr</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>España</t>
+          <t>Francia</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Universidad Del País Vasco</t>
+          <t>Université Paris Iii- Sorbonne Nouvelle</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Enfermeria</t>
+          <t>Estetica</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Autocuidado de la Salud</t>
+          <t>Estéticas del Cine Chileno</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>28176</t>
+          <t>29860</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>ENF425</t>
+          <t>EST6300</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
@@ -629,7 +629,7 @@
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
@@ -644,32 +644,32 @@
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Si</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>No aplica</t>
+          <t>Loreto Massicot</t>
         </is>
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>No aplica</t>
+          <t>Realizado</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>Pregrado</t>
+          <t>Magister</t>
         </is>
       </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>Enfermería</t>
+          <t>no aplica</t>
         </is>
       </c>
       <c r="W2" t="inlineStr">
         <is>
-          <t>si</t>
+          <t>no</t>
         </is>
       </c>
       <c r="X2" t="inlineStr">
@@ -726,17 +726,17 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Estéticas del Cine Chileno</t>
+          <t>Folklore chileno</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>29860</t>
+          <t>15309</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>EST6300</t>
+          <t>ESO008</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
@@ -746,12 +746,12 @@
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>Sí</t>
+          <t>No</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
@@ -776,12 +776,12 @@
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>No aplica</t>
+          <t>Realizado</t>
         </is>
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>Magister</t>
+          <t>Pregrado</t>
         </is>
       </c>
       <c r="V3" t="inlineStr">
@@ -808,57 +808,57 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Cécile Juvé</t>
+          <t>IRATI MAGUNAGOITIA IBARGUENGOITIA</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://www.dropbox.com/scl/fi/2ps9xq5w068xrjdpppv3b/certificados_notas_universidad_origen_JUVE_Cecile.pdf?rlkey=k6tdbssxu60ujapldrt2b6g6d&amp;st=qktkmrtu&amp;dl=0</t>
+          <t>https://www.dropbox.com/scl/fi/wdr7mmp1uawkqyoz6ftgu/Expediente-acad-mico-Irati-Magunagoitia.pdf?rlkey=1azd83tm5at2jry9x4zthoded&amp;st=79ih5b5p&amp;dl=0</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1185373</t>
+          <t>1185454</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>cecile.juve@sorbonne-nouvelle.fr</t>
+          <t>iratimagunagoitia@gmail.com</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>cecile.juve@sorbonne-nouvelle.fr</t>
+          <t>iratimagunagoitia@gmail.com</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Francia</t>
+          <t>España</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Université Paris Iii- Sorbonne Nouvelle</t>
+          <t>Universidad Del País Vasco</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Estetica</t>
+          <t>Enfermeria</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Folklore chileno</t>
+          <t>Autocuidado de la Salud</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>15309</t>
+          <t>28176</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>ESO008</t>
+          <t>ENF425</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
@@ -868,32 +868,32 @@
       </c>
       <c r="N4" t="inlineStr">
         <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
           <t>No</t>
         </is>
       </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>Si</t>
-        </is>
-      </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>Loreto Massicot</t>
+          <t>No aplica</t>
         </is>
       </c>
       <c r="T4" t="inlineStr">
@@ -908,12 +908,12 @@
       </c>
       <c r="V4" t="inlineStr">
         <is>
-          <t>no aplica</t>
+          <t>Enfermería</t>
         </is>
       </c>
       <c r="W4" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>si</t>
         </is>
       </c>
       <c r="X4" t="inlineStr">
@@ -1020,7 +1020,7 @@
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>No aplica</t>
         </is>
       </c>
       <c r="U5" t="inlineStr">
@@ -1142,7 +1142,7 @@
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>No aplica</t>
         </is>
       </c>
       <c r="U6" t="inlineStr">
@@ -1264,25 +1264,139 @@
       </c>
       <c r="T7" t="inlineStr">
         <is>
+          <t>No aplica</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>Pregrado</t>
+        </is>
+      </c>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>Comunicaciones</t>
+        </is>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>si</t>
+        </is>
+      </c>
+      <c r="X7" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Diciembre</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Emma Hayes</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>https://www.dropbox.com/scl/fi/6hhcf9ubc5ttaw1mh20xu/Hayes_Emma_1457184_Official_Transcript.pdf?rlkey=f4h5m2yyoi86e8m5qoygnhjzz&amp;st=qre6dfu6&amp;dl=0</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>1186329</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>hayese27@up.edu</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>hayese27@up.edu</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Estados Unidos</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>IES Abroad</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Desarrollo Sustentable</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sistemas Alimentarios Regenerativos </t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>31900</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>SUS2001</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>Belén Saavedra</t>
+        </is>
+      </c>
+      <c r="T8" t="inlineStr">
+        <is>
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="U7" t="inlineStr">
-        <is>
-          <t>Pregrado</t>
-        </is>
-      </c>
-      <c r="V7" t="inlineStr">
-        <is>
-          <t>Comunicaciones</t>
-        </is>
-      </c>
-      <c r="W7" t="inlineStr">
-        <is>
-          <t>si</t>
-        </is>
-      </c>
-      <c r="X7" t="inlineStr">
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>Pregrado</t>
+        </is>
+      </c>
+      <c r="V8" t="inlineStr"/>
+      <c r="W8" t="inlineStr"/>
+      <c r="X8" t="inlineStr">
         <is>
           <t>Sí</t>
         </is>
@@ -1647,7 +1761,7 @@
         </is>
       </c>
       <c r="R4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S4" t="inlineStr">
         <is>
@@ -3941,7 +4055,7 @@
         </is>
       </c>
       <c r="R30" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S30" t="inlineStr">
         <is>
@@ -4378,7 +4492,7 @@
         </is>
       </c>
       <c r="R35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S35" t="inlineStr">
         <is>
@@ -4387,12 +4501,12 @@
       </c>
       <c r="T35" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="U35" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -6095,12 +6209,12 @@
       </c>
       <c r="T55" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="U55" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -6171,7 +6285,7 @@
         </is>
       </c>
       <c r="R56" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S56" t="inlineStr">
         <is>
@@ -6511,7 +6625,7 @@
         </is>
       </c>
       <c r="R60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S60" t="inlineStr">
         <is>
@@ -7965,12 +8079,12 @@
       </c>
       <c r="T77" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="U77" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -9579,7 +9693,7 @@
         </is>
       </c>
       <c r="R96" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S96" t="inlineStr">
         <is>
@@ -9664,7 +9778,7 @@
         </is>
       </c>
       <c r="R97" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S97" t="inlineStr">
         <is>
@@ -9673,12 +9787,12 @@
       </c>
       <c r="T97" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U97" t="inlineStr">
+        <is>
           <t>0</t>
-        </is>
-      </c>
-      <c r="U97" t="inlineStr">
-        <is>
-          <t>1</t>
         </is>
       </c>
     </row>
@@ -11032,7 +11146,7 @@
         </is>
       </c>
       <c r="R113" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="S113" t="inlineStr">
         <is>
@@ -11041,12 +11155,12 @@
       </c>
       <c r="T113" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="U113" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
     </row>
@@ -11643,7 +11757,7 @@
         </is>
       </c>
       <c r="R120" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S120" t="inlineStr">
         <is>
@@ -11652,12 +11766,12 @@
       </c>
       <c r="T120" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="U120" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -12444,7 +12558,7 @@
         </is>
       </c>
       <c r="R129" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S129" t="inlineStr">
         <is>
@@ -12881,7 +12995,7 @@
         </is>
       </c>
       <c r="R134" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S134" t="inlineStr">
         <is>
@@ -13933,7 +14047,7 @@
         </is>
       </c>
       <c r="R146" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S146" t="inlineStr">
         <is>
@@ -13942,12 +14056,12 @@
       </c>
       <c r="T146" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="U146" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -15144,12 +15258,12 @@
       </c>
       <c r="T160" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="U160" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -15220,7 +15334,7 @@
         </is>
       </c>
       <c r="R161" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S161" t="inlineStr">
         <is>
@@ -15229,12 +15343,12 @@
       </c>
       <c r="T161" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="U161" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -15908,7 +16022,7 @@
         </is>
       </c>
       <c r="R169" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S169" t="inlineStr">
         <is>
@@ -16859,7 +16973,7 @@
         </is>
       </c>
       <c r="R180" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S180" t="inlineStr">
         <is>
@@ -16868,12 +16982,12 @@
       </c>
       <c r="T180" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="U180" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -17454,7 +17568,7 @@
         </is>
       </c>
       <c r="R187" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S187" t="inlineStr">
         <is>
@@ -17709,7 +17823,7 @@
         </is>
       </c>
       <c r="R190" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="S190" t="inlineStr">
         <is>
@@ -17794,7 +17908,7 @@
         </is>
       </c>
       <c r="R191" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S191" t="inlineStr">
         <is>
@@ -17803,12 +17917,12 @@
       </c>
       <c r="T191" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="U191" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -17879,7 +17993,7 @@
         </is>
       </c>
       <c r="R192" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S192" t="inlineStr">
         <is>
@@ -17888,12 +18002,12 @@
       </c>
       <c r="T192" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="U192" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -18304,7 +18418,7 @@
         </is>
       </c>
       <c r="R197" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S197" t="inlineStr">
         <is>
@@ -18313,12 +18427,12 @@
       </c>
       <c r="T197" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="U197" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -18814,7 +18928,7 @@
         </is>
       </c>
       <c r="R203" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="S203" t="inlineStr">
         <is>
@@ -18823,12 +18937,12 @@
       </c>
       <c r="T203" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="U203" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -19874,7 +19988,7 @@
         </is>
       </c>
       <c r="R215" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S215" t="inlineStr">
         <is>
@@ -19883,12 +19997,12 @@
       </c>
       <c r="T215" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="U215" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -34706,7 +34820,7 @@
         </is>
       </c>
       <c r="R383" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S383" t="inlineStr">
         <is>
@@ -34715,12 +34829,12 @@
       </c>
       <c r="T383" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="U383" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -36799,12 +36913,12 @@
       </c>
       <c r="T407" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U407" t="inlineStr">
+        <is>
           <t>0</t>
-        </is>
-      </c>
-      <c r="U407" t="inlineStr">
-        <is>
-          <t>1</t>
         </is>
       </c>
     </row>
@@ -40530,7 +40644,7 @@
         </is>
       </c>
       <c r="R451" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S451" t="inlineStr">
         <is>
@@ -40539,12 +40653,12 @@
       </c>
       <c r="T451" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="U451" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -41890,7 +42004,7 @@
         </is>
       </c>
       <c r="R467" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S467" t="inlineStr">
         <is>
@@ -42060,7 +42174,7 @@
         </is>
       </c>
       <c r="R469" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S469" t="inlineStr">
         <is>
@@ -44052,12 +44166,12 @@
       </c>
       <c r="T492" t="inlineStr">
         <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="U492" t="inlineStr">
+        <is>
           <t>3</t>
-        </is>
-      </c>
-      <c r="U492" t="inlineStr">
-        <is>
-          <t>2</t>
         </is>
       </c>
     </row>
@@ -44217,7 +44331,7 @@
         </is>
       </c>
       <c r="R494" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S494" t="inlineStr">
         <is>
@@ -44302,7 +44416,7 @@
         </is>
       </c>
       <c r="R495" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="S495" t="inlineStr">
         <is>
@@ -44727,7 +44841,7 @@
         </is>
       </c>
       <c r="R500" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S500" t="inlineStr">
         <is>
@@ -44736,12 +44850,12 @@
       </c>
       <c r="T500" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="U500" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -52058,7 +52172,7 @@
         </is>
       </c>
       <c r="R583" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S583" t="inlineStr">
         <is>
@@ -52228,7 +52342,7 @@
         </is>
       </c>
       <c r="R585" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S585" t="inlineStr">
         <is>
@@ -52237,12 +52351,12 @@
       </c>
       <c r="T585" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="U585" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -55656,7 +55770,7 @@
         </is>
       </c>
       <c r="R625" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S625" t="inlineStr">
         <is>
@@ -55745,7 +55859,7 @@
         </is>
       </c>
       <c r="R626" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S626" t="inlineStr">
         <is>
@@ -55754,12 +55868,12 @@
       </c>
       <c r="T626" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="U626" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>8</t>
         </is>
       </c>
     </row>
@@ -56170,7 +56284,7 @@
         </is>
       </c>
       <c r="R631" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S631" t="inlineStr">
         <is>
@@ -56179,12 +56293,12 @@
       </c>
       <c r="T631" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="U631" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -56340,7 +56454,7 @@
         </is>
       </c>
       <c r="R633" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S633" t="inlineStr">
         <is>
@@ -56349,12 +56463,12 @@
       </c>
       <c r="T633" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="U633" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -58906,7 +59020,7 @@
         </is>
       </c>
       <c r="R663" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S663" t="inlineStr">
         <is>
@@ -58915,12 +59029,12 @@
       </c>
       <c r="T663" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="U663" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -58995,7 +59109,7 @@
         </is>
       </c>
       <c r="R664" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S664" t="inlineStr">
         <is>
@@ -59084,7 +59198,7 @@
         </is>
       </c>
       <c r="R665" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S665" t="inlineStr">
         <is>
@@ -59093,12 +59207,12 @@
       </c>
       <c r="T665" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U665" t="inlineStr">
+        <is>
           <t>0</t>
-        </is>
-      </c>
-      <c r="U665" t="inlineStr">
-        <is>
-          <t>1</t>
         </is>
       </c>
     </row>
@@ -62439,12 +62553,12 @@
       </c>
       <c r="T703" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="U703" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -63567,7 +63681,7 @@
         </is>
       </c>
       <c r="R716" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S716" t="inlineStr">
         <is>
@@ -66562,7 +66676,7 @@
         </is>
       </c>
       <c r="R751" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S751" t="inlineStr">
         <is>
@@ -66571,12 +66685,12 @@
       </c>
       <c r="T751" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="U751" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
     </row>

</xml_diff>